<commit_message>
test fonctionnels Register + Connect + URLs
</commit_message>
<xml_diff>
--- a/Tests Fonctionnel.xlsx
+++ b/Tests Fonctionnel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -203,9 +203,6 @@
     <t>http://www.allocine.fr/series/ficheserie_gen_cserie=11939.html</t>
   </si>
   <si>
-    <t>Afficher</t>
-  </si>
-  <si>
     <t>L'Url est intégrée au tableau et une URL minifiée lui est associée</t>
   </si>
   <si>
@@ -218,7 +215,55 @@
     <t>allocine.fr/series/ficheserie_gen_cserie=11939.html</t>
   </si>
   <si>
-    <t>Message de type erreur:</t>
+    <t>Message de type erreur:"URL saisi incorrect"</t>
+  </si>
+  <si>
+    <t>L'utilisateur rentre une URL correct mais l'affichage ne se fait pas</t>
+  </si>
+  <si>
+    <t>Message de type erreur : "Un problème est survenu au moment de l'affichage"</t>
+  </si>
+  <si>
+    <t>URL correcte mais pas d'affichage</t>
+  </si>
+  <si>
+    <t>URL déjà existante</t>
+  </si>
+  <si>
+    <t>L'utilisateur rentre une URL qui a déjà été saisie</t>
+  </si>
+  <si>
+    <t>Message de type erreur: "Votre URL existe déjà"</t>
+  </si>
+  <si>
+    <t>URL correcte mais l'URL minifiée non créée</t>
+  </si>
+  <si>
+    <t>L'utilisateur rentre une URL saisi une URL correcte, qui s'affiche dans le tableau mais l'url minifiée n'est pas crée</t>
+  </si>
+  <si>
+    <t>Message de typeerreur : "L'URL minifiée n'a pas été créée"</t>
+  </si>
+  <si>
+    <t>L'URL disparait du tableau d'affichage</t>
+  </si>
+  <si>
+    <t>La suppression ne fonctionne pas</t>
+  </si>
+  <si>
+    <t>L'utilisateur clique sur le bouton de suppression. L'url disparaît du tableau d'affichage</t>
+  </si>
+  <si>
+    <t>L'utilisateur clique sur le bouton de suppression. L'url  ne disparaît pas du tableau d'affichage</t>
+  </si>
+  <si>
+    <t>L'URL ne disparait pas du tableau d'affichage</t>
+  </si>
+  <si>
+    <t>Gérer URLs</t>
+  </si>
+  <si>
+    <t>Afficher URLs</t>
   </si>
 </sst>
 </file>
@@ -354,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -367,15 +412,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -430,6 +466,43 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,7 +1265,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
     <xdr:pic>
@@ -1225,7 +1298,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9725025" y="6924675"/>
+          <a:off x="9725025" y="10372725"/>
           <a:ext cx="333375" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1238,9 +1311,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
     <xdr:pic>
@@ -1273,7 +1346,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9705975" y="7410450"/>
+          <a:off x="9801225" y="11420475"/>
           <a:ext cx="333375" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1334,17 +1407,17 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Graphique 19" descr="Coche">
+        <xdr:cNvPr id="22" name="Graphique 21" descr="Coche">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DACA4FAF-2B68-48A0-AD68-105CD956EAE1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26CC18B3-52E3-452B-BBB6-69AF7C30BC19}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1369,7 +1442,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9705975" y="7962900"/>
+          <a:off x="9801225" y="13496925"/>
           <a:ext cx="333375" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1382,17 +1455,17 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Graphique 20" descr="Coche">
+        <xdr:cNvPr id="25" name="Graphique 24" descr="Coche">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B753F0DE-B615-4F1A-B686-6E595F839C71}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{861CB96A-6B93-492D-88A1-E9037162DE93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1417,7 +1490,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9696450" y="8553450"/>
+          <a:off x="9791700" y="9534525"/>
           <a:ext cx="333375" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1727,517 +1800,637 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="23"/>
-    <col min="2" max="2" width="19" style="29" customWidth="1"/>
-    <col min="3" max="3" width="19" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28" style="29" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="20"/>
+    <col min="2" max="2" width="19" style="26" customWidth="1"/>
+    <col min="3" max="3" width="19" style="39" customWidth="1"/>
+    <col min="4" max="4" width="29" style="26" customWidth="1"/>
     <col min="5" max="5" width="34.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" style="29" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="20">
+      <c r="A3" s="17">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="11"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="A4" s="18">
         <v>2</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="A5" s="18">
         <v>3</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="17">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="11"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="A7" s="17">
         <v>5</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+      <c r="A8" s="17">
         <v>6</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="11"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
+      <c r="A9" s="17">
         <v>7</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="11"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22">
+      <c r="A10" s="19">
         <v>8</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="13"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
+    <row r="13" spans="1:7" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
         <v>1</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="25" t="s">
         <v>52</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="18"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+      <c r="A14" s="17">
         <v>2</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="11"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
+      <c r="A15" s="17">
         <v>3</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
+      <c r="A16" s="17">
         <v>4</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="11"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="17">
         <v>5</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20">
+      <c r="A18" s="17">
         <v>6</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="11"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
+      <c r="A19" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="29"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
+      <c r="A21" s="14">
         <v>1</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="25" t="s">
         <v>57</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
+        <v>2</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
+      <c r="C22" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
+        <v>3</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <v>4</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="17">
+        <v>5</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="29"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="G27" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>1</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
-        <v>3</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="17" t="s">
+      <c r="D28" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
+        <v>2</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="20">
-        <v>4</v>
-      </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="20">
-        <v>5</v>
-      </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="20">
-        <v>6</v>
-      </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="11"/>
+      <c r="D29" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="34"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="34"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="34"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="30"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A26:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
test fonctionnels Register + Connect + URLs + Redirection
</commit_message>
<xml_diff>
--- a/Tests Fonctionnel.xlsx
+++ b/Tests Fonctionnel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="96">
   <si>
     <t>ID</t>
   </si>
@@ -59,18 +59,12 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Enregistrer</t>
-  </si>
-  <si>
     <t>bob@test.fr  /  #AbcD123  / #AbcD456</t>
   </si>
   <si>
     <t>L'utilisateur n'a pas renseigné le champ email</t>
   </si>
   <si>
-    <t xml:space="preserve"> /  #AbcD123  / #AbcD123</t>
-  </si>
-  <si>
     <t xml:space="preserve">bob@test.fr  /    / </t>
   </si>
   <si>
@@ -242,9 +236,6 @@
     <t>L'utilisateur rentre une URL saisi une URL correcte, qui s'affiche dans le tableau mais l'url minifiée n'est pas crée</t>
   </si>
   <si>
-    <t>Message de typeerreur : "L'URL minifiée n'a pas été créée"</t>
-  </si>
-  <si>
     <t>L'URL disparait du tableau d'affichage</t>
   </si>
   <si>
@@ -264,6 +255,63 @@
   </si>
   <si>
     <t>Afficher URLs</t>
+  </si>
+  <si>
+    <t>Redirection</t>
+  </si>
+  <si>
+    <t>L'utilisateur clique une URL minifiée et est redirigée vars l'URL initiale</t>
+  </si>
+  <si>
+    <t>http://www.urlminimifiee.fr</t>
+  </si>
+  <si>
+    <t>Ouverture  de la page correspondant àl'URL initiale</t>
+  </si>
+  <si>
+    <t>L'URL minifiée n'est pas "liée"</t>
+  </si>
+  <si>
+    <t>L'utilisateur clique sur une URL minifiée mais la redirection ne se fait pas</t>
+  </si>
+  <si>
+    <t>L'URL minifiée redirige sur une page 404</t>
+  </si>
+  <si>
+    <t>L'URL minifiée redirige sur la mauvaise page</t>
+  </si>
+  <si>
+    <t>L'utilisateur clique sur une URL minifiée mais la redirection envoie sur une mauvaise page</t>
+  </si>
+  <si>
+    <t>La redirection se fait sur une autre page que celle du lien de l'URL initiale</t>
+  </si>
+  <si>
+    <t>L'utilisateur clique sur une URL et est renvoyé sur une page 404</t>
+  </si>
+  <si>
+    <t>La redirection se fait sur une page introuvable</t>
+  </si>
+  <si>
+    <t>Le lien de l'URL minifiée n'a pas été crée,donc rien ne se passe . Pas de redirection</t>
+  </si>
+  <si>
+    <t>Enregistrement</t>
+  </si>
+  <si>
+    <t>champ vide avec validation</t>
+  </si>
+  <si>
+    <t>L'utilisateur ne saisi rien dans le champ URL et valide</t>
+  </si>
+  <si>
+    <t>Message de type erreur: "Veuillez saisir une URL"</t>
+  </si>
+  <si>
+    <t>Message de type erreur : "L'URL minifiée n'a pas été créée"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> / #AbcD123  / #AbcD123</t>
   </si>
 </sst>
 </file>
@@ -399,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -467,28 +515,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -503,6 +529,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1312,7 +1347,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
@@ -1408,7 +1443,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
@@ -1456,7 +1491,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
@@ -1491,6 +1526,198 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9791700" y="9534525"/>
+          <a:ext cx="333375" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="333375" cy="333375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Graphique 20" descr="Coche">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD1B4449-FEB8-4CC9-A337-40E865A13ABE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9791700" y="14963775"/>
+          <a:ext cx="333375" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="333375" cy="333375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Graphique 22" descr="Coche">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C34F577-914B-4CC0-A002-0134925B15F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9791700" y="12487275"/>
+          <a:ext cx="333375" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="333375" cy="333375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Graphique 23" descr="Coche">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9492311-D9E9-4AEB-AFBE-F627197D5045}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9801225" y="15030450"/>
+          <a:ext cx="333375" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="333375" cy="333375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Graphique 25" descr="Coche">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DD46DBF-8A5C-4745-BBB6-6443F9943FEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9801225" y="15601950"/>
           <a:ext cx="333375" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1800,32 +2027,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="20"/>
     <col min="2" max="2" width="19" style="26" customWidth="1"/>
-    <col min="3" max="3" width="19" style="39" customWidth="1"/>
+    <col min="3" max="3" width="19" style="31" customWidth="1"/>
     <col min="4" max="4" width="29" style="26" customWidth="1"/>
     <col min="5" max="5" width="34.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="30.5703125" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29"/>
+      <c r="A1" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -1847,7 +2074,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1855,10 +2082,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>54</v>
+        <v>20</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>52</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>6</v>
@@ -1867,7 +2094,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G3" s="8"/>
     </row>
@@ -1876,10 +2103,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>54</v>
+        <v>14</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>52</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>8</v>
@@ -1888,7 +2115,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G4" s="7"/>
     </row>
@@ -1897,19 +2124,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>52</v>
       </c>
       <c r="D5" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>32</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>34</v>
       </c>
       <c r="G5" s="7"/>
     </row>
@@ -1918,19 +2145,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>54</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>52</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G6" s="8"/>
     </row>
@@ -1939,19 +2166,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>54</v>
+        <v>16</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>52</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G7" s="8"/>
     </row>
@@ -1960,19 +2187,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>54</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>52</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" s="8"/>
     </row>
@@ -1981,19 +2208,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>54</v>
+        <v>25</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>52</v>
       </c>
       <c r="D9" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="22" t="s">
         <v>38</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>40</v>
       </c>
       <c r="G9" s="8"/>
     </row>
@@ -2002,32 +2229,32 @@
         <v>8</v>
       </c>
       <c r="B10" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>23</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="A11" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
@@ -2049,7 +2276,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2057,19 +2284,19 @@
         <v>1</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G13" s="15"/>
     </row>
@@ -2078,16 +2305,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>5</v>
@@ -2099,19 +2326,19 @@
         <v>3</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G15" s="8"/>
     </row>
@@ -2120,19 +2347,19 @@
         <v>4</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G16" s="8"/>
     </row>
@@ -2141,19 +2368,19 @@
         <v>5</v>
       </c>
       <c r="B17" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="22" t="s">
+      <c r="F17" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>44</v>
       </c>
       <c r="G17" s="8"/>
     </row>
@@ -2162,32 +2389,32 @@
         <v>6</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>50</v>
-      </c>
       <c r="F18" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29"/>
+      <c r="A19" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="34"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
@@ -2209,7 +2436,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2217,19 +2444,19 @@
         <v>1</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="F21" s="25" t="s">
         <v>57</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>59</v>
       </c>
       <c r="G21" s="15"/>
     </row>
@@ -2238,19 +2465,19 @@
         <v>2</v>
       </c>
       <c r="B22" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="22" t="s">
+      <c r="F22" s="22" t="s">
         <v>61</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>63</v>
       </c>
       <c r="G22" s="8"/>
     </row>
@@ -2259,19 +2486,19 @@
         <v>3</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="F23" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G23" s="8"/>
     </row>
@@ -2280,157 +2507,259 @@
         <v>4</v>
       </c>
       <c r="B24" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>69</v>
-      </c>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <v>5</v>
       </c>
       <c r="B25" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="17">
+        <v>6</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="34"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>1</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="22" t="s">
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="17">
+        <v>2</v>
+      </c>
+      <c r="B30" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="27" t="s">
+      <c r="C30" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="34"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>1</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="29"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="21" t="s">
+      <c r="E33" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="G33" s="15"/>
+    </row>
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="17">
+        <v>2</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="17">
         <v>3</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="B35" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G35" s="8"/>
+    </row>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
         <v>4</v>
       </c>
-      <c r="F27" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
-        <v>1</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="G28" s="15"/>
-    </row>
-    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
-        <v>2</v>
-      </c>
-      <c r="B29" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="34"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="34"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="34"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="34"/>
+      <c r="B36" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A31:G31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
test fonctionnels rajout de création URLs
</commit_message>
<xml_diff>
--- a/Tests Fonctionnel.xlsx
+++ b/Tests Fonctionnel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="103">
   <si>
     <t>ID</t>
   </si>
@@ -56,9 +56,6 @@
     <t>bob.test.fr  /  #AbcD123  / #AbcD123</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>bob@test.fr  /  #AbcD123  / #AbcD456</t>
   </si>
   <si>
@@ -312,13 +309,37 @@
   </si>
   <si>
     <t xml:space="preserve"> / #AbcD123  / #AbcD123</t>
+  </si>
+  <si>
+    <t>/remove-urls</t>
+  </si>
+  <si>
+    <t>route API</t>
+  </si>
+  <si>
+    <t>/redirect-url</t>
+  </si>
+  <si>
+    <t>Créer URLs</t>
+  </si>
+  <si>
+    <t>/add-urls</t>
+  </si>
+  <si>
+    <t>L'utilisateur a crée une URL, celle-ci s'affiche dans le tableau et l'URL minifiée est créée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.allocine.fr/series/ficheserie_gen_cserie=11939.html  </t>
+  </si>
+  <si>
+    <t>http://www.allocine.fr/series/ficheserie_gen_cserie=11939.html    /   http://www.urlminimifiee.fr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +359,14 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -444,10 +473,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -539,8 +569,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1300,7 +1334,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
     <xdr:pic>
@@ -1346,54 +1380,6 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="333375" cy="333375"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Graphique 17" descr="Coche">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98B6CAF2-0D0D-4F9B-B601-49B81F8683E6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9801225" y="11420475"/>
-          <a:ext cx="333375" cy="333375"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -1443,7 +1429,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
@@ -1491,7 +1477,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
@@ -1539,7 +1525,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
@@ -1587,7 +1573,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
@@ -1635,7 +1621,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
@@ -1683,7 +1669,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333375" cy="333375"/>
@@ -1718,6 +1704,150 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9801225" y="15601950"/>
+          <a:ext cx="333375" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="333375" cy="333375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Graphique 26" descr="Coche">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4892288C-E4BD-4B2B-BA8E-A891D7E3827A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9782175" y="11687175"/>
+          <a:ext cx="333375" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="333375" cy="333375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Graphique 28" descr="Coche">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CAA6704-7E36-48ED-8D0F-B5BC85372A99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9801225" y="11801475"/>
+          <a:ext cx="333375" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="333375" cy="333375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Graphique 30" descr="Coche">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4B61CA6-5A08-43B4-9BB3-779FD973F7C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9782175" y="12401550"/>
           <a:ext cx="333375" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2027,10 +2157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2175,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -2062,7 +2192,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>3</v>
@@ -2074,7 +2204,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2082,10 +2212,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>6</v>
@@ -2094,7 +2224,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3" s="8"/>
     </row>
@@ -2103,10 +2233,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>8</v>
@@ -2115,7 +2245,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="7"/>
     </row>
@@ -2124,19 +2254,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="7"/>
     </row>
@@ -2145,19 +2275,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="8"/>
     </row>
@@ -2166,19 +2296,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" s="8"/>
     </row>
@@ -2187,19 +2317,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" s="8"/>
     </row>
@@ -2208,19 +2338,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="22" t="s">
         <v>37</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>38</v>
       </c>
       <c r="G9" s="8"/>
     </row>
@@ -2229,25 +2359,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="33"/>
@@ -2264,7 +2394,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>3</v>
@@ -2276,7 +2406,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2284,19 +2414,19 @@
         <v>1</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="25" t="s">
         <v>50</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>51</v>
       </c>
       <c r="G13" s="15"/>
     </row>
@@ -2305,16 +2435,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>5</v>
@@ -2326,19 +2456,19 @@
         <v>3</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G15" s="8"/>
     </row>
@@ -2347,19 +2477,19 @@
         <v>4</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="F16" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="8"/>
     </row>
@@ -2368,19 +2498,19 @@
         <v>5</v>
       </c>
       <c r="B17" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="22" t="s">
+      <c r="E17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="F17" s="22" t="s">
         <v>41</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>42</v>
       </c>
       <c r="G17" s="8"/>
     </row>
@@ -2389,25 +2519,25 @@
         <v>6</v>
       </c>
       <c r="B18" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>46</v>
-      </c>
       <c r="E18" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="22" t="s">
         <v>48</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>49</v>
       </c>
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="32" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
@@ -2424,7 +2554,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="D20" s="21" t="s">
         <v>3</v>
@@ -2436,7 +2566,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2444,325 +2574,384 @@
         <v>1</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="E21" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="25" t="s">
-        <v>57</v>
-      </c>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17">
         <v>2</v>
       </c>
       <c r="B22" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="22" t="s">
+      <c r="E22" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="F22" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="22" t="s">
-        <v>61</v>
-      </c>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" s="22" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="D23" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="17">
+        <v>5</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="34"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>1</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
+        <v>3</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="17">
+        <v>6</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="34"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
-        <v>5</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17">
-        <v>6</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="22" t="s">
+      <c r="F31" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>1</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="34"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="G32" s="15"/>
+    </row>
+    <row r="33" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="17">
+        <v>2</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="34"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B35" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="21" t="s">
+      <c r="C35" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E35" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F35" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
+      <c r="G35" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
         <v>1</v>
       </c>
-      <c r="B29" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" s="15"/>
-    </row>
-    <row r="30" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="17">
+      <c r="B36" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36" s="15"/>
+    </row>
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="17">
         <v>2</v>
       </c>
-      <c r="B30" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="G30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="34"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="21" t="s">
+      <c r="B37" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="17">
         <v>3</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="B38" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="17">
         <v>4</v>
       </c>
-      <c r="F32" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
-        <v>1</v>
-      </c>
-      <c r="B33" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="25" t="s">
+      <c r="B39" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F33" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="17">
-        <v>2</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F34" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
-        <v>3</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F35" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
-        <v>4</v>
-      </c>
-      <c r="B36" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="25" t="s">
+      <c r="F39" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="G36" s="8"/>
+      <c r="G39" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A25:G25"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E39" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>